<commit_message>
added nb for supp materials excel
Added a new notebook to generate the excel file uploaded in the supplemental materials.
</commit_message>
<xml_diff>
--- a/processed_files/Williams_2019_PRX_Top25.xlsx
+++ b/processed_files/Williams_2019_PRX_Top25.xlsx
@@ -1151,7 +1151,7 @@
         <v>66</v>
       </c>
       <c r="I6">
-        <v>14.82444230909365</v>
+        <v>14.82444230909354</v>
       </c>
       <c r="J6">
         <v>1.795158889098681</v>
@@ -1698,7 +1698,7 @@
         <v>7.652494853644444</v>
       </c>
       <c r="J23">
-        <v>1.271848031681833</v>
+        <v>1.271848031681832</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2745,7 +2745,7 @@
         <v>72</v>
       </c>
       <c r="I3">
-        <v>120.4872541798959</v>
+        <v>120.487254179895</v>
       </c>
       <c r="J3">
         <v>8.361982268369944</v>
@@ -3321,7 +3321,7 @@
         <v>175</v>
       </c>
       <c r="I21">
-        <v>27.72301751119587</v>
+        <v>27.72301751119566</v>
       </c>
       <c r="J21">
         <v>8.880307448950299</v>
@@ -4102,7 +4102,7 @@
         <v>175</v>
       </c>
       <c r="I19">
-        <v>27.72301751119587</v>
+        <v>27.72301751119566</v>
       </c>
       <c r="J19">
         <v>8.880307448950299</v>
@@ -4166,7 +4166,7 @@
         <v>72</v>
       </c>
       <c r="I21">
-        <v>120.4872541798959</v>
+        <v>120.487254179895</v>
       </c>
       <c r="J21">
         <v>8.361982268369944</v>

</xml_diff>